<commit_message>
Acrescentado "Name" do Use Case
</commit_message>
<xml_diff>
--- a/Descrição_use_cases.xlsx
+++ b/Descrição_use_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Informática\3º Ano\1º Semestre\DSS\Trabalho Prático\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Informática\3º Ano\1º Semestre\DSS\dss-1617\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <r>
       <t xml:space="preserve">  </t>
@@ -98,6 +98,9 @@
   <si>
     <t>Excepção 1               (passo X)
 [caso onde ocorre a excepção]</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -141,13 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D15"/>
+  <dimension ref="A3:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -478,6 +484,11 @@
     <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>0</v>
@@ -551,5 +562,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>